<commit_message>
CCDB-180: Fixed data loader for properties to accept the UNIQUE column. Also fixed the integrationm tests to test this.
</commit_message>
<xml_diff>
--- a/conf-core/src/test/resources/dataloader/properties-test.xlsx
+++ b/conf-core/src/test/resources/dataloader/properties-test.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="100">
   <si>
     <t>HEADER</t>
   </si>
@@ -333,6 +333,15 @@
   </si>
   <si>
     <t>Strings List</t>
+  </si>
+  <si>
+    <t>UNIQUE</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>UNIVERSAL</t>
   </si>
 </sst>
 </file>
@@ -368,9 +377,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -680,9 +690,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -694,12 +706,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1242,7 +1254,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -1262,7 +1274,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -1282,82 +1294,116 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" t="s">
+    <row r="35" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
         <v>70</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C38" t="s">
         <v>71</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D38" t="s">
         <v>90</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F38" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="G38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
         <v>72</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C39" t="s">
         <v>73</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D39" t="s">
         <v>90</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F39" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="G39" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
         <v>74</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C40" t="s">
         <v>75</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D40" t="s">
         <v>89</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E40" t="s">
         <v>7</v>
       </c>
-      <c r="F37" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="F40" t="s">
+        <v>93</v>
+      </c>
+      <c r="G40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
         <v>76</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C41" t="s">
         <v>77</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D41" t="s">
         <v>89</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E41" t="s">
         <v>7</v>
       </c>
-      <c r="F38" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="F41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>